<commit_message>
Anhadiendo roles al excelazo.
</commit_message>
<xml_diff>
--- a/public/Uploads/Recursos/temp-usuarios-sigpad.xlsx
+++ b/public/Uploads/Recursos/temp-usuarios-sigpad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Dropbox\UES\2018\TG\EISI\modelo\notas\DCN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,10 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Listado de Usuarios" sheetId="1" r:id="rId1"/>
-    <sheet name="Roles" sheetId="2" r:id="rId2"/>
+    <sheet name="Roles" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Opciones" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="roles">Roles!$B$2:$D$4</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>idRol</t>
   </si>
@@ -239,6 +242,24 @@
   </si>
   <si>
     <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Juancito</t>
+  </si>
+  <si>
+    <t>Palaviccini</t>
+  </si>
+  <si>
+    <t>pala1590</t>
   </si>
 </sst>
 </file>
@@ -297,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -305,6 +326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,19 +641,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A2:D4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.5" customWidth="1"/>
     <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="11" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>69</v>
       </c>
@@ -644,77 +668,93 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="6">
+        <f>IFERROR(VLOOKUP($E2,roles,3,FALSE),"")</f>
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1142,15 +1182,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Roles!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E50</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1212,7 @@
     <col min="3" max="3" width="97" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1180,6 +1232,40 @@
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
+      </c>
+      <c r="D2">
+        <f>A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="0">A3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel modificado con roles e instrucciones.
</commit_message>
<xml_diff>
--- a/public/Uploads/Recursos/temp-usuarios-sigpad.xlsx
+++ b/public/Uploads/Recursos/temp-usuarios-sigpad.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
   <si>
     <t>idRol</t>
   </si>
@@ -253,20 +253,78 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Juancito</t>
-  </si>
-  <si>
-    <t>Palaviccini</t>
-  </si>
-  <si>
-    <t>pala1590</t>
+    <t>INSTRUCCIONES</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>No modifique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> el orden de las columnas ni hojas del formato. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2- Solo seleccione valores de las </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>listas desplegables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, otros valores no serán almacenados. </t>
+    </r>
+  </si>
+  <si>
+    <t>3- Solo se tomarán en cuenta las primeras 50 filas de esta hoja.</t>
+  </si>
+  <si>
+    <t>Nombre1 Nombre2</t>
+  </si>
+  <si>
+    <t>Apellido1 Apellido2</t>
+  </si>
+  <si>
+    <t>AA990001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,16 +340,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -314,11 +394,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -327,6 +495,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,21 +833,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.5" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
     <col min="2" max="2" width="22.125" customWidth="1"/>
     <col min="4" max="4" width="11" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="42.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>69</v>
       </c>
@@ -672,15 +865,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6">
         <f>IFERROR(VLOOKUP($E2,roles,3,FALSE),"")</f>
@@ -689,72 +882,90 @@
       <c r="E2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1180,8 +1391,15 @@
       <c r="C100" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Cambio por lista desplegable para el archivo.
</commit_message>
<xml_diff>
--- a/public/Uploads/Recursos/temp-usuarios-sigpad.xlsx
+++ b/public/Uploads/Recursos/temp-usuarios-sigpad.xlsx
@@ -836,7 +836,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -877,10 +877,10 @@
       </c>
       <c r="D2" s="6">
         <f>IFERROR(VLOOKUP($E2,roles,3,FALSE),"")</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>74</v>
@@ -890,7 +890,10 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E3,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="F3" s="10" t="s">
         <v>75</v>
       </c>
@@ -898,7 +901,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E4,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="F4" s="12" t="s">
         <v>76</v>
       </c>
@@ -908,6 +914,10 @@
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
+      <c r="D5" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E5,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="F5" s="12" t="s">
         <v>77</v>
       </c>
@@ -917,6 +927,10 @@
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
+      <c r="D6" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E6,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15"/>
     </row>
@@ -924,288 +938,464 @@
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
+      <c r="D7" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E7,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
+      <c r="D8" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E8,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
+      <c r="D9" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E9,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
+      <c r="D10" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E10,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
+      <c r="D11" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E11,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
+      <c r="D12" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E12,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
+      <c r="D13" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E13,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
+      <c r="D14" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E14,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
+      <c r="D15" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E15,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E16,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E17,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E18,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E19,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E20,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E21,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E22,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E23,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E24,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E25,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E26,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E27,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E28,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E29,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E30,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E31,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E32,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E33,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E34,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E35,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E36,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E37,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E38,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E39,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E40,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E41,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E42,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E43,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E44,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E45,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E46,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E47,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E48,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E49,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="6" t="str">
+        <f>IFERROR(VLOOKUP($E50,roles,3,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>

</xml_diff>